<commit_message>
IMPORTANT: changed method by which hydrophobicity is calculated, affecting cutoff of homologues that are too polar to really be TMDs --> need to add a separate cutoff for each dataset, because BB is very different from SP! finished gather_pretty_alignments (NOW STABLE!) added more hydrophobicity scales to excel file added double-check regarding the number of proteins after slicing OMPdb dataset, because ~3000 homologues seem to be missing somewhere...
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/hydrophobicity_scales.xlsx
+++ b/korbinian/examples/settings/hydrophobicity_scales.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Ile</t>
   </si>
@@ -163,13 +163,37 @@
   </si>
   <si>
     <t>1aa</t>
+  </si>
+  <si>
+    <t>Elazar</t>
+  </si>
+  <si>
+    <t>Elazar, A. A., Weinstein, J., Biran, I., Fridman, Y., Bibi, E., &amp; Fleishman, S. J. (2016). Mutational scanning reveals the determinants of protein insertion and association energetics in the plasma membrane. Journal of Chemical Information and Modeling, 53(9), 1689–1699. http://doi.org/10.1017/CBO9781107415324.004</t>
+  </si>
+  <si>
+    <t>Hopp-Woods</t>
+  </si>
+  <si>
+    <t>Cornette</t>
+  </si>
+  <si>
+    <t>Eisenberg</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Janin</t>
+  </si>
+  <si>
+    <t>Engelman(GES)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +206,12 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,13 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,24 +546,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -540,8 +574,11 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -557,212 +594,485 @@
       <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-0.17</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="G4" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-0.13</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-0.12</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-3.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-1.23</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.49</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.54</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-3.1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-0.9</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="K6" s="3">
+        <v>-0.6</v>
+      </c>
+      <c r="L6" s="3">
+        <v>-9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-3.5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-2.02</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.68</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.83</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-1.8</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-0.74</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="K7" s="3">
+        <v>-0.7</v>
+      </c>
+      <c r="L7" s="3">
+        <v>-8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-0.32</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-1.63</v>
+      </c>
+      <c r="G8" s="3">
+        <v>-2.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.19</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="3">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-0.01</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.58</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-3.2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-0.96</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="K10" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C11" s="1">
         <v>4.5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D11" s="1">
         <v>0.31</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E11" s="1">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="F11" s="1">
+        <v>-1.57</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-1.8</v>
+      </c>
+      <c r="H11" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.38</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="L11" s="3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-3.9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-0.99</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.71</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>-3.1</v>
+      </c>
+      <c r="I12" s="3">
+        <v>-1.5</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="K12" s="3">
+        <v>-1.8</v>
+      </c>
+      <c r="L12" s="3">
+        <v>-8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-1.92</v>
+      </c>
+      <c r="G13" s="3">
+        <v>-1.8</v>
+      </c>
+      <c r="H13" s="3">
+        <v>5.7</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1.06</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-0.1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="G14" s="3">
+        <v>-1.3</v>
+      </c>
+      <c r="H14" s="3">
         <v>4.2</v>
       </c>
-      <c r="D5" s="1">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>-0.31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-0.32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-0.13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.9</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-0.17</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1">
-        <v>-0.4</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-0.01</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-0.7</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-0.8</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-0.13</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-0.9</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1.85</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I14" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="L14" s="3">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1">
-        <v>-1.3</v>
+        <v>-3.5</v>
       </c>
       <c r="D15" s="1">
-        <v>0.94</v>
+        <v>-0.42</v>
       </c>
       <c r="E15" s="1">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="I15" s="3">
+        <v>-0.78</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="K15" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="L15" s="3">
+        <v>-4.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -778,127 +1088,298 @@
       <c r="E16" s="1">
         <v>2.23</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>1.87</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="K16" s="3">
+        <v>-0.3</v>
+      </c>
+      <c r="L16" s="3">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1">
-        <v>-3.2</v>
+        <v>-3.5</v>
       </c>
       <c r="D17" s="1">
-        <v>-0.96</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="E17" s="1">
-        <v>2.06</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.36</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H17" s="3">
+        <v>-2.8</v>
+      </c>
+      <c r="I17" s="3">
+        <v>-0.85</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="K17" s="3">
+        <v>-0.7</v>
+      </c>
+      <c r="L17" s="3">
+        <v>-4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1">
-        <v>-3.5</v>
+        <v>-4.5</v>
       </c>
       <c r="D18" s="1">
-        <v>-2.02</v>
+        <v>-0.81</v>
       </c>
       <c r="E18" s="1">
-        <v>2.68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.58</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I18" s="3">
+        <v>-2.5299999999999998</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="K18" s="3">
+        <v>-1.4</v>
+      </c>
+      <c r="L18" s="3">
+        <v>-12.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1">
-        <v>-3.5</v>
+        <v>-0.8</v>
       </c>
       <c r="D19" s="1">
-        <v>-0.57999999999999996</v>
+        <v>-0.13</v>
       </c>
       <c r="E19" s="1">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.84</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H19" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="I19" s="3">
+        <v>-0.18</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="K19" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1">
-        <v>-3.5</v>
+        <v>-0.7</v>
       </c>
       <c r="D20" s="1">
-        <v>-1.23</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="E20" s="1">
-        <v>3.49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.52</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="G20" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="H20" s="3">
+        <v>-1.9</v>
+      </c>
+      <c r="I20" s="3">
+        <v>-0.05</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K20" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1">
-        <v>-3.5</v>
+        <v>4.2</v>
       </c>
       <c r="D21" s="1">
-        <v>-0.42</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E21" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-0.31</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-0.6</v>
+      </c>
+      <c r="G21" s="3">
+        <v>-1.5</v>
+      </c>
+      <c r="H21" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1.08</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="L21" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C22" s="1">
-        <v>-3.9</v>
+        <v>-0.9</v>
       </c>
       <c r="D22" s="1">
-        <v>-0.99</v>
+        <v>1.85</v>
       </c>
       <c r="E22" s="1">
-        <v>2.71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="F22" s="1">
+        <v>-0.35</v>
+      </c>
+      <c r="G22" s="3">
+        <v>-3.4</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C23" s="1">
-        <v>-4.5</v>
+        <v>-1.3</v>
       </c>
       <c r="D23" s="1">
-        <v>-0.81</v>
+        <v>0.94</v>
       </c>
       <c r="E23" s="1">
-        <v>2.58</v>
+        <v>0.68</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="G23" s="3">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="H23" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.76</v>
+      </c>
+      <c r="K23" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="L23" s="3">
+        <v>-0.7</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A4:E23">
+    <sortCondition ref="B4:B23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added LIPS hydrophobicity scales updated parse ompdb
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/hydrophobicity_scales.xlsx
+++ b/korbinian/examples/settings/hydrophobicity_scales.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Ile</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Arg</t>
   </si>
   <si>
-    <t>Scale taken from the Chimera docs. https://www.cgl.ucsf.edu/chimera/docs/UsersGuide/midas/hydrophob.html</t>
-  </si>
-  <si>
     <t>Kyte J, Doolittle RF. J Mol Biol. 1982 May 5;157(1):105-32.</t>
   </si>
   <si>
@@ -187,6 +184,39 @@
   </si>
   <si>
     <t>Engelman(GES)</t>
+  </si>
+  <si>
+    <t>LIPS_border</t>
+  </si>
+  <si>
+    <t>LIPS_center</t>
+  </si>
+  <si>
+    <t>Moon CP, Fleming KG. Proc Natl Acad Sci USA. 2011 Jun 21;108(25):10174-7, supplementary data.</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://www.cgl.ucsf.edu/chimera/docs/UsersGuide/midas/hydrophob.html</t>
+  </si>
+  <si>
+    <t>elife-12125-supp1-v3, column c.</t>
+  </si>
+  <si>
+    <t>Extracted by Bo Zeng from LIPS perl code.</t>
+  </si>
+  <si>
+    <t>Adamian, L., &amp; Liang, J. (2006). Prediction of transmembrane helix orientation in polytopic membrane proteins. BMC Structural Biology, 6, 13. http://doi.org/10.1186/1472-6807-6-13</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -234,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -245,6 +275,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -546,82 +578,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1">
         <v>1.8</v>
@@ -632,34 +742,43 @@
       <c r="E4" s="1">
         <v>0.11</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <v>-0.5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>0.2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0.62</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>0.74</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>0.3</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0.71</v>
+      </c>
+      <c r="O4">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>2.5</v>
@@ -670,34 +789,43 @@
       <c r="E5" s="1">
         <v>-0.13</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
+        <v>0.49</v>
+      </c>
+      <c r="G5" s="1">
         <v>-0.12</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>-1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>0.91</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>0.9</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="O5">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1">
         <v>-3.5</v>
@@ -708,34 +836,43 @@
       <c r="E6" s="1">
         <v>3.49</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
+        <v>2.95</v>
+      </c>
+      <c r="G6" s="1">
         <v>1.54</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>-3.1</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>-0.9</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>0.62</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>-0.6</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <v>-9.1999999999999993</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>1.2</v>
+      </c>
+      <c r="O6">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>-3.5</v>
@@ -746,34 +883,43 @@
       <c r="E7" s="1">
         <v>2.68</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
+        <v>1.64</v>
+      </c>
+      <c r="G7" s="1">
         <v>1.83</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>-1.8</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>-0.74</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>0.62</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>-0.7</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>-8.1999999999999993</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0.9</v>
+      </c>
+      <c r="O7">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
         <v>2.8</v>
@@ -784,34 +930,43 @@
       <c r="E8" s="1">
         <v>-0.32</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="G8" s="1">
         <v>-1.63</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>-2.5</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>1.19</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>0.88</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>0.5</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>1.57</v>
+      </c>
+      <c r="O8">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1">
         <v>-0.4</v>
@@ -822,34 +977,43 @@
       <c r="E9" s="1">
         <v>0.74</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
+        <v>1.72</v>
+      </c>
+      <c r="G9" s="1">
         <v>1.58</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
       </c>
       <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
         <v>0.48</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>0.72</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>0.3</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0.48</v>
+      </c>
+      <c r="O9">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1">
         <v>-3.2</v>
@@ -860,34 +1024,43 @@
       <c r="E10" s="1">
         <v>2.06</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
+        <v>4.76</v>
+      </c>
+      <c r="G10" s="1">
         <v>1.85</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>-0.5</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>0.5</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>-0.4</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>0.78</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>-0.1</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="3">
         <v>-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>0.82</v>
+      </c>
+      <c r="O10">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1">
         <v>4.5</v>
@@ -898,34 +1071,43 @@
       <c r="E11" s="1">
         <v>-0.6</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
+        <v>-1.56</v>
+      </c>
+      <c r="G11" s="1">
         <v>-1.57</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>-1.8</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>4.8</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>1.38</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>0.88</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>0.7</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="O11">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1">
         <v>-3.9</v>
@@ -936,34 +1118,43 @@
       <c r="E12" s="1">
         <v>2.71</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
+        <v>5.39</v>
+      </c>
+      <c r="G12" s="1">
         <v>1.51</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>-3.1</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>-1.5</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>0.52</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>-1.8</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <v>-8.8000000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>2.38</v>
+      </c>
+      <c r="O12">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1">
         <v>3.8</v>
@@ -974,34 +1165,43 @@
       <c r="E13" s="1">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
+        <v>-1.81</v>
+      </c>
+      <c r="G13" s="1">
         <v>-1.92</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>-1.8</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>5.7</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>1.06</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>0.85</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>0.5</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>1.18</v>
+      </c>
+      <c r="O13">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1">
         <v>1.9</v>
@@ -1012,34 +1212,43 @@
       <c r="E14" s="1">
         <v>-0.1</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
+        <v>-0.76</v>
+      </c>
+      <c r="G14" s="1">
         <v>-0.8</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>-1.3</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>4.2</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>0.64</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>0.85</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>0.4</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>1.38</v>
+      </c>
+      <c r="O14">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1">
         <v>-3.5</v>
@@ -1050,34 +1259,43 @@
       <c r="E15" s="1">
         <v>2.0499999999999998</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
+        <v>3.47</v>
+      </c>
+      <c r="G15" s="1">
         <v>1.28</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>0.2</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>-0.5</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>-0.78</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>0.63</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L15" s="3">
         <v>-0.5</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <v>-4.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>0.96</v>
+      </c>
+      <c r="O15">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1">
         <v>-1.6</v>
@@ -1088,34 +1306,43 @@
       <c r="E16" s="1">
         <v>2.23</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
+        <v>-1.52</v>
+      </c>
+      <c r="G16" s="1">
         <v>1.87</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>0</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>-2.2000000000000002</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>0.12</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>0.64</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <v>-0.3</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>0.99</v>
+      </c>
+      <c r="O16">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1">
         <v>-3.5</v>
@@ -1126,34 +1353,43 @@
       <c r="E17" s="1">
         <v>2.36</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
+        <v>3.01</v>
+      </c>
+      <c r="G17" s="1">
         <v>0.97</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>0.2</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>-2.8</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>-0.85</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>0.62</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L17" s="3">
         <v>-0.7</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M17" s="3">
         <v>-4.0999999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>0.61</v>
+      </c>
+      <c r="O17">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1">
         <v>-4.5</v>
@@ -1164,34 +1400,43 @@
       <c r="E18" s="1">
         <v>2.58</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
+        <v>3.71</v>
+      </c>
+      <c r="G18" s="1">
         <v>0.79</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>3</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>1.4</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>-2.5299999999999998</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <v>0.64</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <v>-1.4</v>
       </c>
-      <c r="L18" s="3">
+      <c r="M18" s="3">
         <v>-12.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>1.47</v>
+      </c>
+      <c r="O18">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1">
         <v>-0.8</v>
@@ -1202,34 +1447,43 @@
       <c r="E19" s="1">
         <v>0.84</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
+        <v>1.83</v>
+      </c>
+      <c r="G19" s="1">
         <v>0.09</v>
       </c>
-      <c r="G19" s="3">
+      <c r="H19" s="3">
         <v>0.3</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>-0.5</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>-0.18</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>0.66</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L19" s="3">
         <v>-0.1</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M19" s="3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>0.69</v>
+      </c>
+      <c r="O19">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1">
         <v>-0.7</v>
@@ -1240,34 +1494,43 @@
       <c r="E20" s="1">
         <v>0.52</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
+        <v>1.78</v>
+      </c>
+      <c r="G20" s="1">
         <v>0.83</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3">
         <v>-0.4</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>-1.9</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>-0.05</v>
       </c>
-      <c r="J20" s="3">
+      <c r="K20" s="3">
         <v>0.7</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L20" s="3">
         <v>-0.2</v>
       </c>
-      <c r="L20" s="3">
+      <c r="M20" s="3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>0.72</v>
+      </c>
+      <c r="O20">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1">
         <v>4.2</v>
@@ -1278,34 +1541,43 @@
       <c r="E21" s="1">
         <v>-0.31</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
+        <v>-0.78</v>
+      </c>
+      <c r="G21" s="1">
         <v>-0.6</v>
       </c>
-      <c r="G21" s="3">
+      <c r="H21" s="3">
         <v>-1.5</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>4.7</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>1.08</v>
       </c>
-      <c r="J21" s="3">
+      <c r="K21" s="3">
         <v>0.86</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L21" s="3">
         <v>0.6</v>
       </c>
-      <c r="L21" s="3">
+      <c r="M21" s="3">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>0.98</v>
+      </c>
+      <c r="O21">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1">
         <v>-0.9</v>
@@ -1316,34 +1588,43 @@
       <c r="E22" s="1">
         <v>0.3</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22">
+        <v>-0.38</v>
+      </c>
+      <c r="G22" s="1">
         <v>-0.35</v>
       </c>
-      <c r="G22" s="3">
+      <c r="H22" s="3">
         <v>-3.4</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>1</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>0.81</v>
       </c>
-      <c r="J22" s="3">
+      <c r="K22" s="3">
         <v>0.85</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="3">
         <v>0.3</v>
       </c>
-      <c r="L22" s="3">
+      <c r="M22" s="3">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="O22">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1">
         <v>-1.3</v>
@@ -1354,26 +1635,35 @@
       <c r="E23" s="1">
         <v>0.68</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="G23" s="1">
         <v>0.84</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <v>3.2</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>0.26</v>
       </c>
-      <c r="J23" s="3">
+      <c r="K23" s="3">
         <v>0.76</v>
       </c>
-      <c r="K23" s="3">
+      <c r="L23" s="3">
         <v>-0.4</v>
       </c>
-      <c r="L23" s="3">
+      <c r="M23" s="3">
         <v>-0.7</v>
+      </c>
+      <c r="N23">
+        <v>1.23</v>
+      </c>
+      <c r="O23">
+        <v>0.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various compatibility fixes added check for older files
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/hydrophobicity_scales.xlsx
+++ b/korbinian/examples/settings/hydrophobicity_scales.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python_modules\korbinian\korbinian\examples\settings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="16635" windowHeight="10545"/>
+    <workbookView xWindow="3030" yWindow="120" windowWidth="16635" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>Ile</t>
   </si>
@@ -217,12 +222,27 @@
   </si>
   <si>
     <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>Pilpel Y, Ben-Tal N, &amp; Lancet D (1999) KPROT: A knowledge-based scale for the propensity of residue orientation in transmembrane segments. Application to membrane protein structure prediction11Edited by G. von Heijne. J. Mol. Biol. 294(4):921-935.</t>
+  </si>
+  <si>
+    <t>kPROT_Extracellular</t>
+  </si>
+  <si>
+    <t>kPROT_Central</t>
+  </si>
+  <si>
+    <t>kPROT_Intracellular</t>
+  </si>
+  <si>
+    <t>kPROT_Both termini</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -279,7 +299,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -287,14 +307,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,9 +355,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,7 +392,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,7 +427,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -578,20 +601,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>60</v>
       </c>
@@ -635,7 +658,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -678,8 +701,20 @@
       <c r="O2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -725,8 +760,20 @@
       <c r="O3" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -772,8 +819,20 @@
       <c r="O4">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>0.03</v>
+      </c>
+      <c r="Q4">
+        <v>0.09</v>
+      </c>
+      <c r="R4">
+        <v>0.18</v>
+      </c>
+      <c r="S4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -819,8 +878,20 @@
       <c r="O5">
         <v>1.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>0.53</v>
+      </c>
+      <c r="Q5">
+        <v>0.12</v>
+      </c>
+      <c r="R5">
+        <v>0.61</v>
+      </c>
+      <c r="S5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -866,8 +937,20 @@
       <c r="O6">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>1.35</v>
+      </c>
+      <c r="Q6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R6">
+        <v>1.23</v>
+      </c>
+      <c r="S6">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -913,8 +996,20 @@
       <c r="O7">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>1.01</v>
+      </c>
+      <c r="Q7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R7">
+        <v>1.33</v>
+      </c>
+      <c r="S7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -960,8 +1055,20 @@
       <c r="O8">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>0.41</v>
+      </c>
+      <c r="Q8">
+        <v>0.16</v>
+      </c>
+      <c r="R8">
+        <v>0.12</v>
+      </c>
+      <c r="S8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1007,8 +1114,20 @@
       <c r="O9">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>0.02</v>
+      </c>
+      <c r="Q9">
+        <v>0.05</v>
+      </c>
+      <c r="R9">
+        <v>0.33</v>
+      </c>
+      <c r="S9">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1054,8 +1173,20 @@
       <c r="O10">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>0.21</v>
+      </c>
+      <c r="Q10">
+        <v>0.69</v>
+      </c>
+      <c r="R10">
+        <v>0.21</v>
+      </c>
+      <c r="S10">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1101,8 +1232,20 @@
       <c r="O11">
         <v>1.88</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>0.34</v>
+      </c>
+      <c r="Q11">
+        <v>0.12</v>
+      </c>
+      <c r="R11">
+        <v>0.09</v>
+      </c>
+      <c r="S11">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1148,8 +1291,20 @@
       <c r="O12">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>0.85</v>
+      </c>
+      <c r="Q12">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="R12">
+        <v>0.66</v>
+      </c>
+      <c r="S12">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1195,8 +1350,20 @@
       <c r="O13">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>0.11</v>
+      </c>
+      <c r="Q13">
+        <v>0.26</v>
+      </c>
+      <c r="R13">
+        <v>0.17</v>
+      </c>
+      <c r="S13">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -1242,8 +1409,20 @@
       <c r="O14">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q14">
+        <v>0.39</v>
+      </c>
+      <c r="R14">
+        <v>0.32</v>
+      </c>
+      <c r="S14">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1289,8 +1468,20 @@
       <c r="O15">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>0.69</v>
+      </c>
+      <c r="Q15">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="R15">
+        <v>0.75</v>
+      </c>
+      <c r="S15">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1336,8 +1527,20 @@
       <c r="O16">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>0.16</v>
+      </c>
+      <c r="Q16">
+        <v>0.66</v>
+      </c>
+      <c r="R16">
+        <v>0.75</v>
+      </c>
+      <c r="S16">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1383,8 +1586,20 @@
       <c r="O17">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>0.78</v>
+      </c>
+      <c r="Q17">
+        <v>0.83</v>
+      </c>
+      <c r="R17">
+        <v>0.39</v>
+      </c>
+      <c r="S17">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1430,8 +1645,20 @@
       <c r="O18">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>0.53</v>
+      </c>
+      <c r="Q18">
+        <v>0.84</v>
+      </c>
+      <c r="R18">
+        <v>0.44</v>
+      </c>
+      <c r="S18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1477,8 +1704,20 @@
       <c r="O19">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>0.11</v>
+      </c>
+      <c r="Q19">
+        <v>0.22</v>
+      </c>
+      <c r="R19">
+        <v>0.41</v>
+      </c>
+      <c r="S19">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1524,8 +1763,20 @@
       <c r="O20">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>0.03</v>
+      </c>
+      <c r="Q20">
+        <v>0.03</v>
+      </c>
+      <c r="R20">
+        <v>0.43</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1571,8 +1822,20 @@
       <c r="O21">
         <v>1.77</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>0.27</v>
+      </c>
+      <c r="Q21">
+        <v>0.31</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1618,8 +1881,20 @@
       <c r="O22">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>0.25</v>
+      </c>
+      <c r="Q22">
+        <v>0.65</v>
+      </c>
+      <c r="R22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S22">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -1664,6 +1939,18 @@
       </c>
       <c r="O23">
         <v>0.94</v>
+      </c>
+      <c r="P23">
+        <v>0.18</v>
+      </c>
+      <c r="Q23">
+        <v>0.7</v>
+      </c>
+      <c r="R23">
+        <v>0.26</v>
+      </c>
+      <c r="S23">
+        <v>0.23</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1968,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1693,7 +1980,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>